<commit_message>
Fixed footprint for mosfets
P and N channel switching mosfet footprints were incorrect with respect to schematic symbol, flipping gate and source
</commit_message>
<xml_diff>
--- a/Power Distribution Unit 2019 BOM.xlsx
+++ b/Power Distribution Unit 2019 BOM.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TannerOleksiuk\Documents\GitHub\PDU2019\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uvichybrid\Documents\GitHub\PDU2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BAB39461-0D74-4710-82AB-695F19FF2672}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10215" xr2:uid="{EEAE26A0-BBDF-496F-9D7F-FFF146187249}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10215"/>
   </bookViews>
   <sheets>
     <sheet name="Power Distribution Unit 2019" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="180">
   <si>
     <t>Comment</t>
   </si>
@@ -562,12 +561,15 @@
   </si>
   <si>
     <t xml:space="preserve"> WM3801-ND</t>
+  </si>
+  <si>
+    <t>Reset relays</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -956,11 +958,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F33B35A3-4F5E-46FB-AB16-A0AEF5E1DC7E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1345,7 +1347,7 @@
         <v>67</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>31</v>
+        <v>179</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>68</v>

</xml_diff>